<commit_message>
Updated model comparsion table
</commit_message>
<xml_diff>
--- a/models_comprasion.xlsx
+++ b/models_comprasion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://campuscvut-my.sharepoint.com/personal/bimkaond_cvut_cz/Documents/Plocha/Python/GraphPrediction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\OneDrive - České vysoké učení technické v Praze\Plocha\Python\GraphPrediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{667963C4-9CD9-4518-A2CB-CCB76FA769C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2486168B-8F46-4FE5-80EA-3260067F36C5}"/>
+  <xr:revisionPtr revIDLastSave="527" documentId="8_{667963C4-9CD9-4518-A2CB-CCB76FA769C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D409F1CD-F008-44ED-8498-B0F5F8A73390}"/>
   <bookViews>
-    <workbookView xWindow="29100" yWindow="75" windowWidth="24915" windowHeight="14670" xr2:uid="{5AFF6D73-1E5C-4C87-B0A2-B487B8C711A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5AFF6D73-1E5C-4C87-B0A2-B487B8C711A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="36">
   <si>
     <t>LSTM</t>
   </si>
@@ -120,6 +120,27 @@
   </si>
   <si>
     <t>added dropout</t>
+  </si>
+  <si>
+    <t>comp_2</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>24_11_2020</t>
+  </si>
+  <si>
+    <t>28_11_2020</t>
+  </si>
+  <si>
+    <t>23_11_2020</t>
+  </si>
+  <si>
+    <t>21_11_2020</t>
+  </si>
+  <si>
+    <t>20_11_2020</t>
   </si>
 </sst>
 </file>
@@ -141,15 +162,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -306,11 +339,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -336,6 +382,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,6 +548,206 @@
         <a:xfrm>
           <a:off x="10868025" y="4010026"/>
           <a:ext cx="4673600" cy="1257742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>20707</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>34235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>278138</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>161648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB4E66F9-DAD9-489F-AE78-27CE99AEBF25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10860571" y="6950213"/>
+          <a:ext cx="4295203" cy="1386508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>31060</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>72473</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>155090</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>162117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE465188-D256-43EB-B7D4-A2E60D0A9430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10870924" y="5383696"/>
+          <a:ext cx="4161802" cy="1342389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>31059</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>31060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>449508</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DFE9A2F-C4F2-40BD-BBD5-77908EE11A77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10870923" y="8551794"/>
+          <a:ext cx="5067063" cy="1169918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>1120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70AD86DA-B4B3-4B66-8AFB-CBF01DB65F5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10582275" y="9991725"/>
+          <a:ext cx="2511425" cy="715495"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -805,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E11BD4F-9902-4F20-87BF-8B6AB8B32554}">
-  <dimension ref="C3:X30"/>
+  <dimension ref="C3:X62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P67" sqref="P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,10 +1069,13 @@
     <col min="6" max="6" width="11.08984375" customWidth="1"/>
     <col min="7" max="7" width="10.90625" customWidth="1"/>
     <col min="8" max="8" width="11.08984375" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
     <col min="10" max="10" width="15.26953125" customWidth="1"/>
-    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" customWidth="1"/>
     <col min="18" max="18" width="14.08984375" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" customWidth="1"/>
+    <col min="21" max="21" width="11.36328125" customWidth="1"/>
+    <col min="22" max="22" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:24" x14ac:dyDescent="0.35">
@@ -866,7 +1120,9 @@
       <c r="W4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="3:24" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
@@ -910,7 +1166,9 @@
       <c r="W5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
@@ -955,7 +1213,9 @@
       <c r="W6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X6" s="1"/>
+      <c r="X6" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.35">
       <c r="D7" s="1" t="s">
@@ -997,7 +1257,9 @@
       <c r="W7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X7" s="1"/>
+      <c r="X7" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="3:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D8" s="8" t="s">
@@ -1039,7 +1301,9 @@
       <c r="W8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X8" s="1"/>
+      <c r="X8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="3:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="D9" s="6" t="s">
@@ -1081,7 +1345,9 @@
       <c r="W9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X9" s="1"/>
+      <c r="X9" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
@@ -1227,7 +1493,9 @@
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
       <c r="S14" s="13"/>
-      <c r="T14" s="14"/>
+      <c r="T14" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="3:24" x14ac:dyDescent="0.35">
       <c r="D15" s="1" t="s">
@@ -1300,28 +1568,28 @@
       <c r="T16" s="17"/>
     </row>
     <row r="17" spans="4:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="22">
         <v>1.7000000000000001E-4</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="21">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="21">
         <v>1.92E-4</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="21">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="21">
         <v>2.0100000000000001E-4</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="21">
         <v>1.0023000000000001E-2</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="21" t="s">
         <v>22</v>
       </c>
       <c r="L17" s="15"/>
@@ -1405,28 +1673,28 @@
       <c r="T19" s="17"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.35">
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="23">
         <v>1.121E-3</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="23">
         <v>2.06E-2</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="23">
         <v>1.7520000000000001E-3</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="23">
         <v>2.9100000000000001E-2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="23">
         <v>1.3829000000000001E-3</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="23">
         <v>2.52E-2</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="23" t="s">
         <v>22</v>
       </c>
       <c r="L20" s="15"/>
@@ -1513,7 +1781,9 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
-      <c r="T23" s="14"/>
+      <c r="T23" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="4:20" x14ac:dyDescent="0.35">
       <c r="D24" s="1" t="s">
@@ -1747,7 +2017,7 @@
       <c r="J30" s="1">
         <v>3.8899999999999997E-2</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K30" s="24" t="s">
         <v>22</v>
       </c>
       <c r="L30" s="18"/>
@@ -1760,6 +2030,1025 @@
       <c r="S30" s="19"/>
       <c r="T30" s="20"/>
     </row>
+    <row r="31" spans="4:20" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="4"/>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="4:20" x14ac:dyDescent="0.35">
+      <c r="D32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1.2899999999999999E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2.392E-2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1.97E-3</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3.2759999999999997E-2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1.6800000000000001E-3</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="12"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4.46E-4</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4.9399999999999997E-4</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.4899000000000001E-2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>5.3399999999999997E-4</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1.5879999999999998E-2</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="15"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="17"/>
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.3960000000000001E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2.53E-2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1.9189999999999999E-3</v>
+      </c>
+      <c r="H34" s="1">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1.632E-3</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="15"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="17"/>
+    </row>
+    <row r="35" spans="4:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D35" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="21">
+        <v>2.6689999999999998E-4</v>
+      </c>
+      <c r="F35" s="21">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="G35" s="21">
+        <v>2.544E-4</v>
+      </c>
+      <c r="H35" s="21">
+        <v>1.031E-2</v>
+      </c>
+      <c r="I35" s="21">
+        <v>1.8599999999999999E-4</v>
+      </c>
+      <c r="J35" s="21">
+        <v>8.7229999999999999E-3</v>
+      </c>
+      <c r="K35" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="17"/>
+    </row>
+    <row r="36" spans="4:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1.31E-3</v>
+      </c>
+      <c r="F36" s="6">
+        <v>2.47E-2</v>
+      </c>
+      <c r="G36" s="6">
+        <v>2.1220000000000002E-3</v>
+      </c>
+      <c r="H36" s="6">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1.7899999999999999E-3</v>
+      </c>
+      <c r="J36" s="6">
+        <v>3.0759999999999999E-2</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="15"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="17"/>
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2.2070000000000002E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3.5590000000000001E-3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="I37" s="1">
+        <v>2.1120000000000002E-3</v>
+      </c>
+      <c r="J37" s="1">
+        <v>3.3189999999999997E-2</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="15"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="17"/>
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1.4009999999999999E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2.3570000000000001E-2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1.897E-3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>3.0360000000000002E-2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1.7080000000000001E-3</v>
+      </c>
+      <c r="J38" s="1">
+        <v>3.0970000000000001E-2</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="15"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="17"/>
+    </row>
+    <row r="39" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.694E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2.7949999999999999E-2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H39" s="1">
+        <v>3.6990000000000002E-2</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2.0939999999999999E-3</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3.227E-2</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="18"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="20"/>
+    </row>
+    <row r="40" spans="4:21" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="4"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1.645E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2.69E-2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2.2420000000000001E-3</v>
+      </c>
+      <c r="H41" s="1">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1.818E-3</v>
+      </c>
+      <c r="J41" s="1">
+        <v>3.031E-2</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="12"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U41" s="14"/>
+    </row>
+    <row r="42" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2.0396999999999999E-4</v>
+      </c>
+      <c r="F42" s="1">
+        <v>8.8900000000000003E-3</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2.476E-4</v>
+      </c>
+      <c r="H42" s="1">
+        <v>8.6269999999999993E-3</v>
+      </c>
+      <c r="I42" s="1">
+        <v>2.8899999999999998E-4</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1.085E-2</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="15"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="17"/>
+    </row>
+    <row r="43" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1.6130000000000001E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1.3699999999999999E-3</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2.64E-2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1.5150000000000001E-3</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2.7449999999999999E-2</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="15"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="17"/>
+    </row>
+    <row r="44" spans="4:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="8">
+        <v>1.92E-4</v>
+      </c>
+      <c r="F44" s="8">
+        <v>9.3519999999999992E-3</v>
+      </c>
+      <c r="G44" s="8">
+        <v>2.8180000000000002E-4</v>
+      </c>
+      <c r="H44" s="8">
+        <v>1.077E-2</v>
+      </c>
+      <c r="I44" s="8">
+        <v>2.163E-4</v>
+      </c>
+      <c r="J44" s="8">
+        <v>1.06E-2</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L44" s="15"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="17"/>
+    </row>
+    <row r="45" spans="4:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1.696E-3</v>
+      </c>
+      <c r="F45" s="6">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="G45" s="6">
+        <v>2.1900000000000001E-3</v>
+      </c>
+      <c r="H45" s="6">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="I45" s="6">
+        <v>1.8699999999999999E-3</v>
+      </c>
+      <c r="J45" s="6">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45" s="15"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="17"/>
+    </row>
+    <row r="46" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2.0300000000000001E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3.1099999999999999E-2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2.532E-3</v>
+      </c>
+      <c r="H46" s="1">
+        <v>3.8850000000000003E-2</v>
+      </c>
+      <c r="I46" s="1">
+        <v>2.2100000000000002E-3</v>
+      </c>
+      <c r="J46" s="1">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L46" s="15"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="17"/>
+    </row>
+    <row r="47" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1.895E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2.0100000000000001E-3</v>
+      </c>
+      <c r="H47" s="1">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1.48E-3</v>
+      </c>
+      <c r="J47" s="1">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L47" s="15"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="17"/>
+    </row>
+    <row r="48" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2.1770000000000001E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="G48" s="1">
+        <v>2.32E-3</v>
+      </c>
+      <c r="H48" s="1">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="I48" s="1">
+        <v>2.5500000000000002E-3</v>
+      </c>
+      <c r="J48" s="1">
+        <v>3.85E-2</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L48" s="18"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="20"/>
+    </row>
+    <row r="49" spans="4:21" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="4"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>8.7500000000000002E-4</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1.7690000000000001E-2</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1.08E-3</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="I50" s="1">
+        <v>1.31E-3</v>
+      </c>
+      <c r="J50" s="1">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L50" s="12"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2">
+        <v>8.7109999999999998E-5</v>
+      </c>
+      <c r="F51" s="1">
+        <v>4.4600000000000004E-3</v>
+      </c>
+      <c r="G51" s="2">
+        <v>8.1580000000000002E-5</v>
+      </c>
+      <c r="H51" s="1">
+        <v>4.3299999999999996E-3</v>
+      </c>
+      <c r="I51" s="1">
+        <v>1.27E-4</v>
+      </c>
+      <c r="J51" s="1">
+        <v>5.2199999999999998E-3</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L51" s="15"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="17"/>
+    </row>
+    <row r="52" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="1">
+        <v>8.3900000000000001E-4</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1.7260000000000001E-2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1.07E-3</v>
+      </c>
+      <c r="H52" s="1">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1.31E-3</v>
+      </c>
+      <c r="J52" s="1">
+        <v>2.4400000000000002E-2</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L52" s="15"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+      <c r="T52" s="16"/>
+      <c r="U52" s="17"/>
+    </row>
+    <row r="53" spans="4:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D53" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1.0900000000000001E-4</v>
+      </c>
+      <c r="F53" s="8">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="G53" s="8">
+        <v>1.3200000000000001E-4</v>
+      </c>
+      <c r="H53" s="8">
+        <v>6.3E-3</v>
+      </c>
+      <c r="I53" s="8">
+        <v>1.6899999999999999E-4</v>
+      </c>
+      <c r="J53" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L53" s="15"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="17"/>
+    </row>
+    <row r="54" spans="4:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F54" s="6">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="G54" s="6">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="H54" s="6">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="I54" s="6">
+        <v>1.58E-3</v>
+      </c>
+      <c r="J54" s="6">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L54" s="15"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="16"/>
+      <c r="U54" s="17"/>
+    </row>
+    <row r="55" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1.25E-3</v>
+      </c>
+      <c r="H55" s="1">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="I55" s="1">
+        <v>1.48E-3</v>
+      </c>
+      <c r="J55" s="1">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L55" s="15"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="17"/>
+    </row>
+    <row r="56" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="1">
+        <v>9.3800000000000003E-4</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="H56" s="1">
+        <v>2.24E-2</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="J56" s="1">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L56" s="15"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="17"/>
+    </row>
+    <row r="57" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1.09E-3</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="H57" s="1">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I57" s="1">
+        <v>1.66E-3</v>
+      </c>
+      <c r="J57" s="1">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L57" s="18"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="19"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="19"/>
+      <c r="S57" s="19"/>
+      <c r="T57" s="19"/>
+      <c r="U57" s="20"/>
+    </row>
+    <row r="58" spans="4:21" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>7.182E-3</v>
+      </c>
+      <c r="F59" s="1">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="G59" s="1">
+        <v>6.8780000000000004E-3</v>
+      </c>
+      <c r="H59" s="1">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="I59" s="1">
+        <v>7.0829999999999999E-3</v>
+      </c>
+      <c r="J59" s="1">
+        <v>5.5399999999999998E-2</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L59" s="12"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="13"/>
+      <c r="U59" s="14"/>
+    </row>
+    <row r="60" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="1">
+        <v>3.0209999999999998E-3</v>
+      </c>
+      <c r="F60" s="1">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="G60" s="1">
+        <v>3.9560000000000003E-3</v>
+      </c>
+      <c r="H60" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I60" s="1">
+        <v>2.9420000000000002E-3</v>
+      </c>
+      <c r="J60" s="1">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L60" s="15"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="16"/>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+      <c r="Q60" s="16"/>
+      <c r="R60" s="16"/>
+      <c r="S60" s="16"/>
+      <c r="T60" s="16"/>
+      <c r="U60" s="17"/>
+    </row>
+    <row r="61" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1">
+        <v>4.078E-3</v>
+      </c>
+      <c r="F61" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G61" s="1">
+        <v>4.0829999999999998E-3</v>
+      </c>
+      <c r="H61" s="1">
+        <v>4.41E-2</v>
+      </c>
+      <c r="I61" s="1">
+        <v>5.0109999999999998E-3</v>
+      </c>
+      <c r="J61" s="1">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L61" s="15"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="16"/>
+      <c r="R61" s="16"/>
+      <c r="S61" s="16"/>
+      <c r="T61" s="16"/>
+      <c r="U61" s="17"/>
+    </row>
+    <row r="62" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="D62" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="25">
+        <v>4.078E-3</v>
+      </c>
+      <c r="F62" s="25">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G62" s="25">
+        <v>4.0829999999999998E-3</v>
+      </c>
+      <c r="H62" s="25">
+        <v>4.419E-2</v>
+      </c>
+      <c r="I62" s="25">
+        <v>5.0109999999999998E-3</v>
+      </c>
+      <c r="J62" s="25">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L62" s="18"/>
+      <c r="M62" s="19"/>
+      <c r="N62" s="19"/>
+      <c r="O62" s="19"/>
+      <c r="P62" s="19"/>
+      <c r="Q62" s="19"/>
+      <c r="R62" s="19"/>
+      <c r="S62" s="19"/>
+      <c r="T62" s="19"/>
+      <c r="U62" s="20"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1769,6 +3058,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BB4A5DEBB3C39B41B2C977608B031513" ma:contentTypeVersion="12" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="e335dfb80c6e6aa700d587729ed40fe5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="11b3ca6c-9a68-4285-a8b8-5e60b2655545" xmlns:ns4="6cdfea00-299d-40e0-a4a3-06bf7212faa0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a4f162329493b58d7d63ccb4e34a2d" ns3:_="" ns4:_="">
     <xsd:import namespace="11b3ca6c-9a68-4285-a8b8-5e60b2655545"/>
@@ -1985,15 +3283,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2001,6 +3290,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D06D365-3EB5-4F20-AFA8-EEF17C635D0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F12BF5F2-C90E-4AD4-8E53-D3528ECD179D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2019,14 +3316,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D06D365-3EB5-4F20-AFA8-EEF17C635D0A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D54D1DD-8720-4C80-AAFF-6E84BECC6459}">
   <ds:schemaRefs>

</xml_diff>